<commit_message>
webapp_model2: round slider update values to step size to avoid reset of output summary, included time step in "entire_forecast" reactive variable --> button can be clicked several times in a row
</commit_message>
<xml_diff>
--- a/Benchmark_Results.xlsx
+++ b/Benchmark_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Webapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA784C72-5967-4E3F-9423-CC38FD52C6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D676217-F222-4C32-A482-1CAF842A77C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{7C7C4834-B17F-491C-B4F8-1BA18C3EB9BB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Huber Loss</t>
   </si>
@@ -44,61 +44,31 @@
     <t>Mean Absolute Error (MAE)</t>
   </si>
   <si>
-    <t>27.52 MW</t>
-  </si>
-  <si>
     <t>Mean Squared Error (MSE)</t>
   </si>
   <si>
-    <t>2941.27 MW²</t>
-  </si>
-  <si>
     <t>Benchmark</t>
   </si>
   <si>
-    <t>25.67 MW</t>
-  </si>
-  <si>
-    <t>2681.88 MW²</t>
-  </si>
-  <si>
-    <t>28.11 MW</t>
-  </si>
-  <si>
-    <t>3077.00 MW²</t>
-  </si>
-  <si>
-    <t>0.1607 MW</t>
-  </si>
-  <si>
-    <t>0.0617 MW²</t>
-  </si>
-  <si>
     <t>with real capacities</t>
   </si>
   <si>
     <t>normalised</t>
   </si>
   <si>
-    <t>0.1522 MW</t>
-  </si>
-  <si>
-    <t>0.0571 MW²</t>
-  </si>
-  <si>
-    <t>0.1623 MW</t>
-  </si>
-  <si>
-    <t>0.0619 MW²</t>
-  </si>
-  <si>
-    <t>0.1212 MW</t>
-  </si>
-  <si>
-    <t>0.0287 MW²</t>
-  </si>
-  <si>
     <t>Model (100.000 data points, with cut-off of 0.01 values)</t>
+  </si>
+  <si>
+    <t>Root Mean Squared Error (RMSE)</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>MW²</t>
+  </si>
+  <si>
+    <t>unit</t>
   </si>
 </sst>
 </file>
@@ -470,22 +440,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B7E56C7-1B1A-4724-9AEF-72C8F1A0C666}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D7:D9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -497,7 +470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -511,108 +484,150 @@
         <v>27.65</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>27.52</v>
+      </c>
+      <c r="D4">
+        <v>25.67</v>
+      </c>
+      <c r="E4">
+        <v>28.11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C5">
+        <v>2941.27</v>
+      </c>
+      <c r="D5">
+        <v>2681.88</v>
+      </c>
+      <c r="E5">
+        <v>3077</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>54.23</v>
+      </c>
+      <c r="D6">
+        <v>51.79</v>
+      </c>
+      <c r="E6">
+        <v>55.47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>3.09E-2</v>
+      </c>
+      <c r="D8">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>3.09E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.16070000000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.1522</v>
+      </c>
+      <c r="E9">
+        <v>0.1623</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>6.1699999999999998E-2</v>
+      </c>
+      <c r="D10">
+        <v>5.7099999999999998E-2</v>
+      </c>
+      <c r="E10">
+        <v>6.1899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>0.24840000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.24879999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1.43E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0.1212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>2.87E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>3.09E-2</v>
-      </c>
-      <c r="D7">
-        <v>2.8500000000000001E-2</v>
-      </c>
-      <c r="E7">
-        <v>3.09E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>1.43E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
+      <c r="C16">
+        <v>0.1694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>